<commit_message>
cleaning files and restructuing the project
</commit_message>
<xml_diff>
--- a/log-analyzer/src/output/log_analysis.xlsx
+++ b/log-analyzer/src/output/log_analysis.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Failed Entries" sheetId="2" r:id="rId2"/>
     <sheet name="Service Entries" sheetId="3" r:id="rId3"/>
     <sheet name="Log Level Entries" sheetId="4" r:id="rId4"/>
+    <sheet name=" Error Messages count " sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>date_time</t>
   </si>
@@ -62,6 +63,15 @@
   </si>
   <si>
     <t>2023-03-01 09:11:00</t>
+  </si>
+  <si>
+    <t>2023-03-01 09:12:01</t>
+  </si>
+  <si>
+    <t>2023-03-01 09:13:01</t>
+  </si>
+  <si>
+    <t>2023-03-01 09:44:01</t>
   </si>
   <si>
     <t>ServiceA</t>
@@ -142,7 +152,7 @@
     <t>[{'date_time': '2023-03-01 08:15:27', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Started processing request #123'}, {'date_time': '2023-03-01 08:15:29', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Completed request #123 in 2ms'}, {'date_time': '2023-03-01 08:40:05', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Cleaned up temporary files'}]</t>
   </si>
   <si>
-    <t>[{'date_time': '2023-03-01 08:15:28', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 08:35:10', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 09:00:00', 'service_name': 'ServiceB', 'log_level': 'INFO', 'message': 'Started job X'}, {'date_time': '2023-03-01 09:00:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}]</t>
+    <t>[{'date_time': '2023-03-01 08:15:28', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 08:35:10', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 09:00:00', 'service_name': 'ServiceB', 'log_level': 'INFO', 'message': 'Started job X'}, {'date_time': '2023-03-01 09:00:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:12:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:13:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:44:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}]</t>
   </si>
   <si>
     <t>[{'date_time': '2023-03-01 08:20:05', 'service_name': 'ServiceC', 'log_level': 'WARN', 'message': 'Disk usage is at 85%'}, {'date_time': '2023-03-01 09:10:00', 'service_name': 'ServiceC', 'log_level': 'WARN', 'message': 'Low memory'}]</t>
@@ -157,7 +167,13 @@
     <t>[{'date_time': '2023-03-01 08:15:27', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Started processing request #123'}, {'date_time': '2023-03-01 08:15:29', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Completed request #123 in 2ms'}, {'date_time': '2023-03-01 08:40:05', 'service_name': 'ServiceA', 'log_level': 'INFO', 'message': 'Cleaned up temporary files'}, {'date_time': '2023-03-01 08:44:11', 'service_name': 'ServiceD', 'log_level': 'INFO', 'message': 'Heartbeat check'}, {'date_time': '2023-03-01 09:00:00', 'service_name': 'ServiceB', 'log_level': 'INFO', 'message': 'Started job X'}]</t>
   </si>
   <si>
-    <t>[{'date_time': '2023-03-01 08:15:28', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 08:35:10', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 09:00:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}]</t>
+    <t>[{'date_time': '2023-03-01 08:15:28', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 08:35:10', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Null pointer exception'}, {'date_time': '2023-03-01 09:00:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:12:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:13:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}, {'date_time': '2023-03-01 09:44:01', 'service_name': 'ServiceB', 'log_level': 'ERROR', 'message': 'Job X failed to start'}]</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -515,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,13 +556,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -554,13 +570,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -568,13 +584,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -582,13 +598,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -596,13 +612,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -610,13 +626,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -624,13 +640,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -638,13 +654,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -652,13 +668,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -666,13 +682,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -680,13 +696,55 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -709,12 +767,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -735,65 +793,65 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -814,54 +872,91 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>